<commit_message>
Benchmark, Version 1 sent to JLCPCB for manufacture
</commit_message>
<xml_diff>
--- a/PCB/Waveform Generator/assembly/CPL.xlsx
+++ b/PCB/Waveform Generator/assembly/CPL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nanodyn-my.sharepoint.com/personal/nicholas_nanodyn_co_za/Documents/Desktop/GIT repository/Waveform-generator/PCB/Waveform Generator/assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="11_6804885380716C36F28B90806F9BEBDF0CF3BBDA" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{20685EF8-816F-4AB1-B4F0-230876FFA79C}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="11_6804885380716C36F28B90806F9BEBDF0CF3BBDA" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{819BC612-039E-48BF-A9C9-FDFDCB1DD782}"/>
   <bookViews>
-    <workbookView xWindow="-6135" yWindow="-12720" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9855" yWindow="-16770" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1254,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E83" sqref="A83:E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1285,14 +1285,14 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
+      <c r="A2" s="3">
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>180</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -1302,65 +1302,65 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
+      <c r="A3" s="3">
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>182</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>183</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
+      <c r="A4" s="3">
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>185</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
+      <c r="A5" s="3">
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>186</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>187</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>189</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -1370,167 +1370,167 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>190</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>152</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
+      <c r="A10" s="3">
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>196</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="2" t="s">
-        <v>35</v>
+      <c r="A11" s="3">
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>197</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>198</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="2" t="s">
-        <v>37</v>
+      <c r="A12" s="3">
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>199</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>200</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="2" t="s">
-        <v>40</v>
+      <c r="A13" s="3">
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>38</v>
+        <v>201</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>41</v>
+        <v>202</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="2" t="s">
-        <v>42</v>
+      <c r="A14" s="3">
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>203</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>43</v>
+        <v>204</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="2" t="s">
-        <v>44</v>
+      <c r="A15" s="3">
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>205</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>46</v>
+        <v>206</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="2" t="s">
-        <v>47</v>
+      <c r="A16" s="3">
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>48</v>
+        <v>207</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>49</v>
+        <v>208</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>11</v>
@@ -1540,14 +1540,14 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="2" t="s">
-        <v>50</v>
+      <c r="A17" s="3">
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>51</v>
+        <v>209</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>52</v>
+        <v>210</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>11</v>
@@ -1557,48 +1557,48 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="2" t="s">
-        <v>53</v>
+      <c r="A18" s="3">
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>54</v>
+        <v>211</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>52</v>
+        <v>212</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="2" t="s">
-        <v>55</v>
+      <c r="A19" s="3">
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>56</v>
+        <v>213</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>57</v>
+        <v>214</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="2" t="s">
-        <v>58</v>
+      <c r="A20" s="3">
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>59</v>
+        <v>215</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>60</v>
+        <v>216</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>11</v>
@@ -1608,14 +1608,14 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="2" t="s">
-        <v>62</v>
+      <c r="A21" s="3">
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>63</v>
+        <v>217</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>64</v>
+        <v>218</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>11</v>
@@ -1625,31 +1625,31 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="2" t="s">
-        <v>65</v>
+      <c r="A22" s="3">
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>67</v>
+        <v>219</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="2" t="s">
-        <v>68</v>
+      <c r="A23" s="3">
+        <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>69</v>
+        <v>220</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>70</v>
+        <v>221</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>11</v>
@@ -1659,48 +1659,48 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="2" t="s">
-        <v>71</v>
+      <c r="A24" s="3">
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>72</v>
+        <v>222</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>73</v>
+        <v>223</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="2" t="s">
-        <v>77</v>
+      <c r="A26" s="3">
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>78</v>
+        <v>225</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>79</v>
+        <v>226</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>11</v>
@@ -1710,31 +1710,31 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="2" t="s">
-        <v>80</v>
+      <c r="A27" s="3">
+        <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>56</v>
+        <v>227</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>81</v>
+        <v>228</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="2" t="s">
-        <v>82</v>
+      <c r="A28" s="3">
+        <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>63</v>
+        <v>229</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>83</v>
+        <v>230</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>11</v>
@@ -1744,31 +1744,31 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="2" t="s">
-        <v>84</v>
+      <c r="A29" s="3">
+        <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>85</v>
+        <v>231</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>86</v>
+        <v>232</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="2" t="s">
-        <v>87</v>
+      <c r="A30" s="3">
+        <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>88</v>
+        <v>233</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>89</v>
+        <v>234</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>11</v>
@@ -1778,133 +1778,133 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="2" t="s">
-        <v>90</v>
+      <c r="A31" s="3">
+        <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>91</v>
+        <v>233</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>92</v>
+        <v>235</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="3">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="3">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="2" t="s">
+    <row r="37" spans="1:5">
+      <c r="A37" s="3">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="2">
-        <v>180</v>
-      </c>
-    </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="2" t="s">
-        <v>111</v>
+      <c r="A38" s="3">
+        <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>112</v>
+        <v>244</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>113</v>
+        <v>245</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>11</v>
@@ -1914,14 +1914,14 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="2" t="s">
-        <v>114</v>
+      <c r="A39" s="3">
+        <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>115</v>
+        <v>246</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>116</v>
+        <v>247</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>11</v>
@@ -1931,184 +1931,184 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="2" t="s">
-        <v>117</v>
+      <c r="A40" s="3">
+        <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>118</v>
+        <v>248</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>119</v>
+        <v>249</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>119</v>
+        <v>10</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B43" s="2">
-        <v>90.5</v>
+        <v>17</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>129</v>
+        <v>22</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>131</v>
+        <v>23</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>132</v>
+        <v>24</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>133</v>
+        <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>134</v>
+        <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>135</v>
+        <v>46</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>136</v>
+        <v>47</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>137</v>
+        <v>48</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>138</v>
+        <v>49</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>137</v>
+        <v>51</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>140</v>
+        <v>52</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="2" t="s">
-        <v>141</v>
+        <v>53</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>142</v>
+        <v>54</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>143</v>
+        <v>52</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E49" s="2">
-        <v>90</v>
+      <c r="E49" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
-        <v>144</v>
+        <v>55</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>145</v>
+        <v>56</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>146</v>
+        <v>57</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>11</v>
@@ -2119,13 +2119,13 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>149</v>
+        <v>60</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>11</v>
@@ -2136,81 +2136,81 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
-        <v>150</v>
+        <v>62</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>151</v>
+        <v>63</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>152</v>
+        <v>64</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
-        <v>153</v>
+        <v>65</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>155</v>
+        <v>67</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E53" s="2">
-        <v>270</v>
+      <c r="E53" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
-        <v>156</v>
+        <v>68</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>157</v>
+        <v>69</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E54" s="2">
-        <v>0</v>
+      <c r="E54" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
-        <v>159</v>
+        <v>71</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>160</v>
+        <v>72</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>161</v>
+        <v>73</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E55" s="2">
-        <v>90</v>
+      <c r="E55" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
-        <v>162</v>
+        <v>6</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>163</v>
+        <v>25</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>164</v>
+        <v>26</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>11</v>
@@ -2221,115 +2221,115 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="2" t="s">
-        <v>165</v>
+        <v>74</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>166</v>
+        <v>75</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>167</v>
+        <v>76</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E57" s="2">
-        <v>90</v>
+      <c r="E57" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="2" t="s">
-        <v>168</v>
+        <v>77</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>169</v>
+        <v>78</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>170</v>
+        <v>79</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E58" s="2">
-        <v>180</v>
+      <c r="E58" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="2" t="s">
-        <v>171</v>
+        <v>80</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>172</v>
+        <v>56</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E59" s="2">
-        <v>180</v>
+      <c r="E59" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="2" t="s">
-        <v>174</v>
+        <v>82</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>175</v>
+        <v>63</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>176</v>
+        <v>83</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E60" s="2">
-        <v>90</v>
+      <c r="E60" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="2" t="s">
-        <v>177</v>
+        <v>84</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>178</v>
+        <v>85</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>179</v>
+        <v>86</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E61" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="3">
-        <v>1</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="3">
-        <v>2</v>
-      </c>
       <c r="B63" s="2" t="s">
-        <v>182</v>
+        <v>91</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>183</v>
+        <v>92</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>11</v>
@@ -2339,48 +2339,48 @@
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="3">
-        <v>3</v>
+      <c r="A64" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>184</v>
+        <v>94</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>185</v>
+        <v>95</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="3">
-        <v>4</v>
+      <c r="A65" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>186</v>
+        <v>97</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>187</v>
+        <v>98</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="3">
-        <v>5</v>
+      <c r="A66" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>188</v>
+        <v>100</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>189</v>
+        <v>101</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>11</v>
@@ -2390,14 +2390,14 @@
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="3">
-        <v>6</v>
+      <c r="A67" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>190</v>
+        <v>27</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>152</v>
+        <v>28</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>11</v>
@@ -2407,201 +2407,201 @@
       </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="3">
-        <v>7</v>
+      <c r="A68" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>192</v>
+        <v>104</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="3">
-        <v>8</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="3">
-        <v>9</v>
+      <c r="A70" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>195</v>
+        <v>27</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>196</v>
+        <v>31</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="3">
-        <v>10</v>
+      <c r="A71" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>197</v>
+        <v>33</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>198</v>
+        <v>34</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E71" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="3">
-        <v>11</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E72" s="2" t="s">
+    <row r="78" spans="1:5">
+      <c r="A78" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="3">
-        <v>12</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="3">
-        <v>13</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" s="3">
-        <v>14</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="3">
-        <v>15</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="3">
-        <v>16</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="3">
-        <v>17</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="3">
-        <v>18</v>
+      <c r="A79" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>213</v>
+        <v>118</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>214</v>
+        <v>119</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>11</v>
@@ -2611,99 +2611,99 @@
       </c>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="3">
-        <v>19</v>
+      <c r="A80" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>215</v>
+        <v>121</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>216</v>
+        <v>119</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E80" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B82" s="2">
+        <v>90.5</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="3">
-        <v>20</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="3">
-        <v>21</v>
-      </c>
-      <c r="B82" s="2" t="s">
+    <row r="85" spans="1:5">
+      <c r="A85" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
-      <c r="A83" s="3">
-        <v>22</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
-      <c r="A84" s="3">
-        <v>23</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="3">
-        <v>24</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="C85" s="2" t="s">
-        <v>224</v>
+        <v>135</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>11</v>
@@ -2713,14 +2713,14 @@
       </c>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="3">
-        <v>25</v>
+      <c r="A86" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>225</v>
+        <v>137</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>226</v>
+        <v>138</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>11</v>
@@ -2730,14 +2730,14 @@
       </c>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="3">
-        <v>26</v>
+      <c r="A87" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>227</v>
+        <v>137</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>228</v>
+        <v>140</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>11</v>
@@ -2747,31 +2747,31 @@
       </c>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="3">
-        <v>27</v>
+      <c r="A88" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>229</v>
+        <v>142</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>230</v>
+        <v>143</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E88" s="2" t="s">
-        <v>29</v>
+      <c r="E88" s="2">
+        <v>90</v>
       </c>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="3">
-        <v>28</v>
+      <c r="A89" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>231</v>
+        <v>145</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>232</v>
+        <v>146</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>11</v>
@@ -2781,14 +2781,14 @@
       </c>
     </row>
     <row r="90" spans="1:5">
-      <c r="A90" s="3">
-        <v>29</v>
+      <c r="A90" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>234</v>
+        <v>149</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>11</v>
@@ -2798,14 +2798,14 @@
       </c>
     </row>
     <row r="91" spans="1:5">
-      <c r="A91" s="3">
-        <v>30</v>
+      <c r="A91" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>233</v>
+        <v>151</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>235</v>
+        <v>152</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>11</v>
@@ -2815,156 +2815,156 @@
       </c>
     </row>
     <row r="92" spans="1:5">
-      <c r="A92" s="3">
-        <v>31</v>
+      <c r="A92" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="C92" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E92" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E93" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E94" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E96" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E97" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E98" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E99" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
-      <c r="A93" s="3">
-        <v>32</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
-      <c r="A94" s="3">
-        <v>33</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
-      <c r="A95" s="3">
-        <v>34</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
-      <c r="A96" s="3">
-        <v>35</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
-      <c r="A97" s="3">
-        <v>36</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
-      <c r="A98" s="3">
-        <v>37</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="A99" s="3">
-        <v>38</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
-      <c r="A100" s="3">
-        <v>39</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="D100" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E100" s="2" t="s">
-        <v>12</v>
+      <c r="E100" s="2">
+        <v>90</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -3037,81 +3037,81 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="2" t="s">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>261</v>
+        <v>284</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E105" s="2">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="2" t="s">
-        <v>262</v>
+        <v>285</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>263</v>
+        <v>286</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>264</v>
+        <v>287</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E106" s="2">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E107" s="2">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="2" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>184</v>
+        <v>263</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E108" s="2">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>11</v>
@@ -3122,87 +3122,87 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>274</v>
+        <v>184</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E110" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="2" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E111" s="2">
-        <v>270</v>
+        <v>180</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="2" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E112" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="2" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E113" s="2">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E114" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -3223,6 +3223,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E114">
+    <sortCondition ref="A2:A114"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>